<commit_message>
Se agregan nuevos casos de uso, cesion de contrato nit a nit con cambio de plan pospago empresarial 5.3 y activacion nintendo con nit
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla9\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E16929-F4F3-4115-AAE4-DA20B4BD287E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE788AF3-BA99-4D78-98DB-8A90F071AEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
   <si>
     <t>MSIDN</t>
   </si>
@@ -220,15 +220,6 @@
     <t>3043209819</t>
   </si>
   <si>
-    <t>732111324707276</t>
-  </si>
-  <si>
-    <t>732111324707277</t>
-  </si>
-  <si>
-    <t>3043209863</t>
-  </si>
-  <si>
     <t>3043209868</t>
   </si>
   <si>
@@ -271,37 +262,64 @@
     <t>163908584</t>
   </si>
   <si>
-    <t>3045981670</t>
-  </si>
-  <si>
     <t>732111193278811</t>
   </si>
   <si>
     <t>732111193280551</t>
   </si>
   <si>
-    <t>732111193280544</t>
-  </si>
-  <si>
     <t>3046010569</t>
   </si>
   <si>
-    <t>3046010523</t>
-  </si>
-  <si>
-    <t>732111193280535</t>
-  </si>
-  <si>
-    <t>3046008593</t>
-  </si>
-  <si>
     <t>697979125</t>
   </si>
   <si>
-    <t>LM845504</t>
-  </si>
-  <si>
-    <t>Tigo.2021*</t>
+    <t>3052749177</t>
+  </si>
+  <si>
+    <t>3052754285</t>
+  </si>
+  <si>
+    <t>732111324709512</t>
+  </si>
+  <si>
+    <t>3045987650</t>
+  </si>
+  <si>
+    <t>732111324709673</t>
+  </si>
+  <si>
+    <t>732111324709674</t>
+  </si>
+  <si>
+    <t>3045984556</t>
+  </si>
+  <si>
+    <t>732111324709675</t>
+  </si>
+  <si>
+    <t>3052754289</t>
+  </si>
+  <si>
+    <t>3046008586</t>
+  </si>
+  <si>
+    <t>732111324709676</t>
+  </si>
+  <si>
+    <t>732111193278871</t>
+  </si>
+  <si>
+    <t>cliente nit a nit</t>
+  </si>
+  <si>
+    <t>996850563</t>
+  </si>
+  <si>
+    <t>940606921</t>
+  </si>
+  <si>
+    <t>904344855</t>
   </si>
 </sst>
 </file>
@@ -941,10 +959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -988,13 +1006,13 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1003,10 +1021,10 @@
         <v>25</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>36</v>
@@ -1028,10 +1046,10 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -1051,7 +1069,7 @@
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
@@ -1063,7 +1081,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>50</v>
@@ -1074,7 +1092,7 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -1091,10 +1109,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -1131,19 +1149,19 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>56</v>
@@ -1160,22 +1178,22 @@
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>60</v>
@@ -1189,58 +1207,92 @@
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se realizan ajuste para la captura de evidencias y se ajustas tiempos de ejecución
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla9\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla9\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE788AF3-BA99-4D78-98DB-8A90F071AEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9590C38-FF9A-49E4-849D-90B43312DAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>MSIDN</t>
   </si>
@@ -202,18 +202,12 @@
     <t>81684</t>
   </si>
   <si>
-    <t>1061520830</t>
-  </si>
-  <si>
     <t>00002201108240181684</t>
   </si>
   <si>
     <t>81670</t>
   </si>
   <si>
-    <t>111295346</t>
-  </si>
-  <si>
     <t>00002201108240181670</t>
   </si>
   <si>
@@ -250,76 +244,58 @@
     <t>SIEBEL</t>
   </si>
   <si>
-    <t>309991475</t>
-  </si>
-  <si>
-    <t>491453906</t>
-  </si>
-  <si>
-    <t>270670616</t>
-  </si>
-  <si>
-    <t>163908584</t>
-  </si>
-  <si>
     <t>732111193278811</t>
   </si>
   <si>
-    <t>732111193280551</t>
-  </si>
-  <si>
-    <t>3046010569</t>
-  </si>
-  <si>
-    <t>697979125</t>
-  </si>
-  <si>
-    <t>3052749177</t>
-  </si>
-  <si>
-    <t>3052754285</t>
-  </si>
-  <si>
-    <t>732111324709512</t>
-  </si>
-  <si>
-    <t>3045987650</t>
-  </si>
-  <si>
-    <t>732111324709673</t>
-  </si>
-  <si>
-    <t>732111324709674</t>
-  </si>
-  <si>
-    <t>3045984556</t>
-  </si>
-  <si>
-    <t>732111324709675</t>
-  </si>
-  <si>
-    <t>3052754289</t>
-  </si>
-  <si>
-    <t>3046008586</t>
-  </si>
-  <si>
-    <t>732111324709676</t>
-  </si>
-  <si>
-    <t>732111193278871</t>
-  </si>
-  <si>
     <t>cliente nit a nit</t>
   </si>
   <si>
-    <t>996850563</t>
-  </si>
-  <si>
-    <t>940606921</t>
-  </si>
-  <si>
     <t>904344855</t>
+  </si>
+  <si>
+    <t>3052755808</t>
+  </si>
+  <si>
+    <t>732111324709812</t>
+  </si>
+  <si>
+    <t>3052755811</t>
+  </si>
+  <si>
+    <t>732111324709813</t>
+  </si>
+  <si>
+    <t>3052755812</t>
+  </si>
+  <si>
+    <t>732111324709814</t>
+  </si>
+  <si>
+    <t>3052755815</t>
+  </si>
+  <si>
+    <t>732111324709816</t>
+  </si>
+  <si>
+    <t>841794534</t>
+  </si>
+  <si>
+    <t>543372417</t>
+  </si>
+  <si>
+    <t>922697306</t>
+  </si>
+  <si>
+    <t>121541180</t>
+  </si>
+  <si>
+    <t>850396952</t>
+  </si>
+  <si>
+    <t>29389214</t>
+  </si>
+  <si>
+    <t>105952330</t>
   </si>
 </sst>
 </file>
@@ -391,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -407,6 +383,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -959,10 +936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1006,13 +983,13 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1046,10 +1023,10 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -1057,19 +1034,19 @@
       <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
@@ -1081,7 +1058,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>50</v>
@@ -1092,7 +1069,7 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -1109,10 +1086,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -1125,25 +1102,25 @@
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1152,16 +1129,16 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>56</v>
@@ -1170,10 +1147,10 @@
         <v>57</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1">
@@ -1181,28 +1158,28 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1">
@@ -1210,13 +1187,13 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1">
@@ -1224,16 +1201,16 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1">
@@ -1241,58 +1218,16 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>